<commit_message>
iteration to comply with latest WhizniumDBE standard
</commit_message>
<xml_diff>
--- a/_mdl/IexWdbeBdd_msdd.xlsx
+++ b/_mdl/IexWdbeBdd_msdd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpsitech/doc/msdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D082673-D4BC-4F43-99E0-071C1C7CCCEA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7DC6CD-15C0-544B-89E2-61407DF7444A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="20400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="27580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IexWdbeBdd" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="115">
   <si>
     <t>ImeIMModule.srefIxVBasetype</t>
   </si>
@@ -355,13 +355,31 @@
   </si>
   <si>
     <t>mnfprim</t>
+  </si>
+  <si>
+    <t>IexWdbeBdd v0.9.44</t>
+  </si>
+  <si>
+    <t>ImeIAMUnitPar.end</t>
+  </si>
+  <si>
+    <t>ImeIMModule.end</t>
+  </si>
+  <si>
+    <t>ImeIMUnit.end</t>
+  </si>
+  <si>
+    <t>ImeIMImbuf.end</t>
+  </si>
+  <si>
+    <t>ImeIAMModulePar.end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -381,14 +399,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF3366FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -422,16 +432,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color rgb="FF3366FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1443,36 +1447,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2802,1441 +2802,1557 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="53.5" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="8" style="10" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="36" style="10" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="53.5" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1">
-      <c r="A2" s="5" t="s">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" s="14" customFormat="1">
-      <c r="B3" s="14" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F9" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="B12" s="2" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E14" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D15" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F16" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="2" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F18" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="2" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="2" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F20" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="2" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F21" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="2" t="s">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="9" customFormat="1">
-      <c r="B21" s="9" t="s">
+    <row r="23" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C23" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D23" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:6" s="1" customFormat="1">
-      <c r="C22" s="1" t="s">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
-      <c r="C23" s="2" t="s">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D25" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E25" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="C24" s="1" t="s">
+    <row r="26" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D27" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="C25" s="2" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D28" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
-      <c r="C26" s="2" t="s">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D29" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
-      <c r="C27" s="2" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D30" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
-      <c r="C28" s="2" t="s">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D31" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="29" spans="2:6" s="9" customFormat="1">
-      <c r="B29" s="9" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C33" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D33" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E33" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="2:6" s="1" customFormat="1">
-      <c r="C30" s="1" t="s">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D34" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E34" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
-      <c r="C31" s="2" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D35" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E35" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
-      <c r="C32" s="1" t="s">
+    <row r="36" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D37" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
-      <c r="C33" s="2" t="s">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D38" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
-      <c r="C34" s="2" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C39" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D39" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
-      <c r="C35" s="2" t="s">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D40" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
-      <c r="C36" s="2" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C41" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D41" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="2" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C42" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C43" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E43" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F43" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="2" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C44" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E44" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
-      <c r="B39" s="2" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C45" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D45" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E45" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
-      <c r="B40" s="2" t="s">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C46" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F46" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="2" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C47" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F47" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="2" t="s">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C48" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D48" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F48" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
-      <c r="B43" s="2" t="s">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C49" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F49" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="2" t="s">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C50" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F50" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="2" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D51" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E51" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="2" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C52" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D52" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E52" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="2:6" s="9" customFormat="1">
-      <c r="B47" s="9" t="s">
+    <row r="53" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C53" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D53" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E53" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="2:6" s="1" customFormat="1">
-      <c r="C48" s="1" t="s">
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D54" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E54" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="C49" s="2" t="s">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C55" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D55" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E55" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="C50" s="1" t="s">
+    <row r="56" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D57" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="C51" s="2" t="s">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C58" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D58" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="C52" s="2" t="s">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C59" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D59" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="C53" s="2" t="s">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C60" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D60" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="C54" s="2" t="s">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C61" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D61" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="9" customFormat="1">
-      <c r="B55" s="9" t="s">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C62" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C63" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D63" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E63" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="12"/>
-    </row>
-    <row r="56" spans="1:6" s="1" customFormat="1">
-      <c r="C56" s="1" t="s">
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D64" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E64" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="C57" s="2" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C65" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D65" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E65" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="C58" s="1" t="s">
+    <row r="66" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C67" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D67" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="C59" s="2" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C68" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D68" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="C60" s="2" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C69" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D69" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="C61" s="2" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D70" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="C62" s="2" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D71" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="5" customFormat="1">
-      <c r="A63" s="5" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C72" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B74" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C74" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="7"/>
-    </row>
-    <row r="64" spans="1:6" s="1" customFormat="1">
-      <c r="B64" s="1" t="s">
+      <c r="D74" s="2"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C75" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
-      <c r="B65" s="2" t="s">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B76" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C76" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
-      <c r="B66" s="2" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B77" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C77" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
-      <c r="B67" s="2" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C78" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="2:6" s="1" customFormat="1">
-      <c r="B68" s="1" t="s">
+    <row r="79" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C80" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D80" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E80" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F80" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
-      <c r="B69" s="2" t="s">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D81" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E81" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="2:6">
-      <c r="B70" s="2" t="s">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B82" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C82" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D82" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E82" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="2:6">
-      <c r="B71" s="2" t="s">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B83" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C83" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D83" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E83" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="2:6">
-      <c r="B72" s="2" t="s">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B84" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C84" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D84" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E84" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:6">
-      <c r="B73" s="2" t="s">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B85" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C85" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D85" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E85" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="2:6">
-      <c r="B74" s="2" t="s">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B86" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C86" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D86" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E86" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:6">
-      <c r="B75" s="2" t="s">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B87" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C87" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D87" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E87" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="76" spans="2:6">
-      <c r="B76" s="2" t="s">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B88" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C88" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D88" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E88" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="2:6">
-      <c r="B77" s="2" t="s">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C89" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E89" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F89" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
-      <c r="B78" s="2" t="s">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B90" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C90" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D90" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E90" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
-      <c r="B79" s="2" t="s">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B91" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C91" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E91" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F91" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="80" spans="2:6">
-      <c r="B80" s="2" t="s">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C92" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D92" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E92" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="2:6">
-      <c r="B81" s="2" t="s">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B93" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C93" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E93" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="F93" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="2:6">
-      <c r="B82" s="2" t="s">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B94" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C94" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E94" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="F94" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:6">
-      <c r="B83" s="2" t="s">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B95" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C95" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D95" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E95" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="2:6" s="9" customFormat="1">
-      <c r="B84" s="9" t="s">
+    <row r="96" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C96" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D96" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="E96" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F84" s="12"/>
-    </row>
-    <row r="85" spans="2:6" s="1" customFormat="1">
-      <c r="C85" s="1" t="s">
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C97" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D97" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E97" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
-      <c r="C86" s="2" t="s">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C98" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D98" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E98" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
-      <c r="C87" s="1" t="s">
+    <row r="99" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C99" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C100" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D100" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
-      <c r="C88" s="2" t="s">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C101" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D101" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="2:6">
-      <c r="C89" s="2" t="s">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C102" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D102" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="2:6">
-      <c r="C90" s="2" t="s">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C103" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D90" s="4" t="s">
+      <c r="D103" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="91" spans="2:6">
-      <c r="C91" s="2" t="s">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C104" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D104" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="92" spans="2:6" s="9" customFormat="1">
-      <c r="B92" s="9" t="s">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C105" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" s="9"/>
+    </row>
+    <row r="106" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C106" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D106" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E92" s="11" t="s">
+      <c r="E106" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F92" s="12"/>
-    </row>
-    <row r="93" spans="2:6" s="1" customFormat="1">
-      <c r="C93" s="1" t="s">
+      <c r="F106" s="8"/>
+    </row>
+    <row r="107" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C107" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D107" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E107" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="2:6">
-      <c r="C94" s="2" t="s">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C108" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D108" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="E108" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="2:6">
-      <c r="C95" s="1" t="s">
+    <row r="109" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C109" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C110" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D110" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="2:6">
-      <c r="C96" s="2" t="s">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C111" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D111" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="2:6">
-      <c r="C97" s="2" t="s">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C112" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D112" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="2:6">
-      <c r="C98" s="2" t="s">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C113" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D113" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="99" spans="2:6">
-      <c r="C99" s="2" t="s">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C114" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D114" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="100" spans="2:6">
-      <c r="B100" s="2" t="s">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C115" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" s="9"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B116" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C116" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E116" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F100" s="3" t="s">
+      <c r="F116" s="11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="2:6">
-      <c r="B101" s="2" t="s">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B117" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C117" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E117" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="102" spans="2:6">
-      <c r="B102" s="2" t="s">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B118" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C118" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D118" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E118" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="2:6">
-      <c r="B103" s="2" t="s">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B119" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C119" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E119" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F119" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="104" spans="2:6">
-      <c r="B104" s="2" t="s">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B120" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C120" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E104" s="5" t="s">
+      <c r="E120" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F104" s="3" t="s">
+      <c r="F120" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="105" spans="2:6">
-      <c r="B105" s="2" t="s">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B121" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C121" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D121" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E105" s="5" t="s">
+      <c r="E121" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F105" s="3" t="s">
+      <c r="F121" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="2:6">
-      <c r="B106" s="2" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B122" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C122" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E106" s="5" t="s">
+      <c r="E122" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F106" s="8" t="s">
+      <c r="F122" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="2:6">
-      <c r="B107" s="2" t="s">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B123" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C123" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E107" s="5" t="s">
+      <c r="E123" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F107" s="3" t="s">
+      <c r="F123" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="108" spans="2:6">
-      <c r="B108" s="2" t="s">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B124" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C124" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D124" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E108" s="5" t="s">
+      <c r="E124" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="109" spans="2:6">
-      <c r="B109" s="2" t="s">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B125" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C125" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D125" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E109" s="5" t="s">
+      <c r="E125" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="2:6" s="9" customFormat="1">
-      <c r="B110" s="9" t="s">
+    <row r="126" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="C126" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D110" s="2" t="s">
+      <c r="D126" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E110" s="11" t="s">
+      <c r="E126" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F110" s="12"/>
-    </row>
-    <row r="111" spans="2:6" s="1" customFormat="1">
-      <c r="C111" s="1" t="s">
+      <c r="F126" s="8"/>
+    </row>
+    <row r="127" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C127" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D127" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="E127" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="2:6">
-      <c r="C112" s="2" t="s">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C128" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D128" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E128" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="2:6">
-      <c r="C113" s="1" t="s">
+    <row r="129" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C129" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C130" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D130" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="2:6">
-      <c r="C114" s="2" t="s">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C131" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D131" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="2:6">
-      <c r="C115" s="2" t="s">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C132" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D132" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="2:6">
-      <c r="C116" s="2" t="s">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C133" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="D133" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="117" spans="2:6">
-      <c r="C117" s="2" t="s">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C134" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D134" s="10">
         <v>38400</v>
       </c>
     </row>
-    <row r="118" spans="2:6" s="9" customFormat="1">
-      <c r="B118" s="9" t="s">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C135" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D135" s="9"/>
+    </row>
+    <row r="136" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="C136" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="D136" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E118" s="11" t="s">
+      <c r="E136" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F118" s="12"/>
-    </row>
-    <row r="119" spans="2:6" s="1" customFormat="1">
-      <c r="C119" s="1" t="s">
+      <c r="F136" s="8"/>
+    </row>
+    <row r="137" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C137" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D137" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="E137" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="2:6">
-      <c r="C120" s="2" t="s">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C138" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D138" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E138" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="2:6">
-      <c r="C121" s="1" t="s">
+    <row r="139" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C139" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C140" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D140" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:6">
-      <c r="C122" s="2" t="s">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C141" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D122" s="2">
+      <c r="D141" s="10">
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="2:6">
-      <c r="C123" s="2" t="s">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C142" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D142" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="2:6">
-      <c r="C124" s="2" t="s">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C143" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D124" s="4" t="s">
+      <c r="D143" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="125" spans="2:6">
-      <c r="C125" s="2" t="s">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C144" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D125" s="2">
+      <c r="D144" s="10">
         <v>38400</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C145" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D145" s="9"/>
+    </row>
+    <row r="146" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B146" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>